<commit_message>
add polonius.next to xlsx
</commit_message>
<xml_diff>
--- a/polonius.next/Book1.xlsx
+++ b/polonius.next/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="13260"/>
+    <workbookView windowWidth="27795" windowHeight="12150"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="56">
   <si>
     <t>stacked borrow</t>
   </si>
@@ -22,12 +22,12 @@
     <t>polonius</t>
   </si>
   <si>
+    <t>polonius + clear_origin</t>
+  </si>
+  <si>
     <t>polonius.next</t>
   </si>
   <si>
-    <t>nll?</t>
-  </si>
-  <si>
     <t>copy1</t>
   </si>
   <si>
@@ -46,10 +46,10 @@
     <t>var b live at</t>
   </si>
   <si>
+    <t>none</t>
+  </si>
+  <si>
     <t>mid</t>
-  </si>
-  <si>
-    <t>none</t>
   </si>
   <si>
     <t>var a defined at</t>
@@ -69,6 +69,11 @@
   <si>
     <t>clear_origin o_a
 var b live at</t>
+  </si>
+  <si>
+    <t>access_origin 'b
+clear_origin 'a
+intro_subset 'b 'a</t>
   </si>
   <si>
     <t xml:space="preserve">push SharedRO(a)
@@ -96,6 +101,11 @@
 var b live at</t>
   </si>
   <si>
+    <t>access_origin 'b
+clear_origin 'a
+TODO</t>
+  </si>
+  <si>
     <t>push Unique(a)</t>
   </si>
   <si>
@@ -120,6 +130,12 @@
 var b live at</t>
   </si>
   <si>
+    <t xml:space="preserve">
+intro_subset L 'a
+clear_origin 'a
+</t>
+  </si>
+  <si>
     <t>loan_issued_at L o_a</t>
   </si>
   <si>
@@ -133,6 +149,11 @@
   </si>
   <si>
     <t>use-1 b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">intro_subset L 'a
+clear_origin 'a
+</t>
   </si>
   <si>
     <t>push  Unique(a)
@@ -143,6 +164,12 @@
   </si>
   <si>
     <t>a = &amp;* b</t>
+  </si>
+  <si>
+    <t>access_origin 'b
+invalidate_origin L
+intro_subset L  'a
+intro_subset 'b L</t>
   </si>
   <si>
     <t>loan_issued_at L o_a
@@ -180,6 +207,13 @@
     <t>clear_origin o_a
 clear all loan of *b
 var b live at</t>
+  </si>
+  <si>
+    <t>access_origin 'b
+clear_origin 'a
+invalidate_origin L
+intro_subset L  'a
+intro_subset 'b L</t>
   </si>
 </sst>
 </file>
@@ -187,10 +221,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -201,102 +235,118 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -322,26 +372,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -360,79 +394,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,97 +568,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,17 +582,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,6 +602,21 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,15 +674,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -650,148 +684,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1135,8 +1169,8 @@
   <sheetPr/>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
@@ -1145,8 +1179,9 @@
     <col min="2" max="2" width="22.2416666666667" customWidth="1"/>
     <col min="3" max="3" width="11.8083333333333" customWidth="1"/>
     <col min="5" max="5" width="17.925" customWidth="1"/>
-    <col min="6" max="6" width="22.5833333333333" customWidth="1"/>
+    <col min="6" max="6" width="7.15" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="22.9333333333333" customWidth="1"/>
+    <col min="8" max="8" width="20.075" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="26" customHeight="1" spans="5:8">
@@ -1159,11 +1194,11 @@
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" ht="28.5" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1184,6 +1219,9 @@
       </c>
       <c r="G2" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1191,10 +1229,10 @@
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -1203,7 +1241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" ht="28.5" spans="1:7">
+    <row r="4" ht="28.5" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -1224,6 +1262,9 @@
       </c>
       <c r="G4" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="28.5" spans="1:7">
@@ -1231,24 +1272,24 @@
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" ht="42.75" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" ht="85.5" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1257,13 +1298,16 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1271,27 +1315,27 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" ht="42.75" spans="1:7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" ht="99.75" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -1300,10 +1344,13 @@
         <v>16</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" ht="28.5" spans="1:7">
@@ -1311,39 +1358,42 @@
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" ht="47" customHeight="1" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" ht="47" customHeight="1" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" ht="28.5" spans="1:7">
@@ -1351,27 +1401,27 @@
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" ht="28.5" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" ht="28.5" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -1385,106 +1435,115 @@
       <c r="G12" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" ht="28.5" spans="1:7">
+      <c r="H12" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" ht="71.25" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" ht="42.75" spans="1:7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" ht="85.5" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" ht="28.5" spans="1:7">
+    <row r="15" ht="71.25" spans="1:7">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" ht="42.75" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" ht="71.25" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" ht="28.5" spans="1:7">
+        <v>54</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" ht="71.25" spans="1:7">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="32">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
@@ -1509,6 +1568,14 @@
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C16:C17"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>